<commit_message>
Completed tests cases 1-8
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ProductsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ProductsModuleTest.xlsx
@@ -1,41 +1,213 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="verifyProductsPage" sheetId="1" r:id="rId1"/>
+    <sheet name="TC_PRODUCTS_001" sheetId="1" r:id="rId1"/>
+    <sheet name="TC_PRODUCTS_002" sheetId="2" r:id="rId2"/>
+    <sheet name="TC_PRODUCTS_004" sheetId="3" r:id="rId3"/>
+    <sheet name="TC_PRODUCTS_005" sheetId="4" r:id="rId4"/>
+    <sheet name="TC_PRODUCTS_006" sheetId="5" r:id="rId5"/>
+    <sheet name="TC_PRODUCTS_007" sheetId="6" r:id="rId6"/>
+    <sheet name="TC_PRODUCTS_008" sheetId="7" r:id="rId7"/>
+    <sheet name="TC_PRODUCTS_009" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>testCaseId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>BreadCrumbsList</t>
   </si>
   <si>
-    <t>TC_PRODUCTS_001</t>
-  </si>
-  <si>
     <t>PIM,Product Master,Products</t>
   </si>
+  <si>
+    <t>Product Name *, Product Number *, Product Description 1, Product Description 2, Product Features, Product Marketing Description, Product Custom Keywords</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Number</t>
+  </si>
+  <si>
+    <t>Product Tabs</t>
+  </si>
+  <si>
+    <t>General Info, Product Images, Item List</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List of Add New Product's Fields </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Asterisk has to be inculded for mandatory fields)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Product Name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Product Number </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Product Description 1, Product Description 2, Product Features, Product Marketing Description, Product Custom Keywords</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">General Info Fields </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Asterisk has to be inculded for mandatory fields)</t>
+    </r>
+  </si>
+  <si>
+    <t>Product Creation Success Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name to be Updated </t>
+  </si>
+  <si>
+    <t>Product Update Success Message</t>
+  </si>
+  <si>
+    <t>Product Removal Success Message</t>
+  </si>
+  <si>
+    <t>AutomationProduct3313</t>
+  </si>
+  <si>
+    <t>New Product saved successfully</t>
+  </si>
+  <si>
+    <t>AutomationProduct3313 Updated</t>
+  </si>
+  <si>
+    <t>Updated Successfully</t>
+  </si>
+  <si>
+    <t>Product deleted successfully</t>
+  </si>
+  <si>
+    <r>
+      <t>Product Images Fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Asterisk has to be inculded for mandatory fields)</t>
+    </r>
+  </si>
+  <si>
+    <t>Action, Image, Image Name</t>
+  </si>
+  <si>
+    <t>Image Desc, Product Image URL, Upload Product Image</t>
+  </si>
+  <si>
+    <r>
+      <t>Add New Product Images Fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Asterisk has to be inculded for mandatory fields)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -82,10 +254,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,7 +322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,10 +354,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,7 +388,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,33 +563,289 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="45">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3313</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3313</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Products module, Dependency issue is pending
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ProductsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ProductsModuleTest.xlsx
@@ -4,24 +4,31 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
-    <sheet name="TC_PRODUCTS_001" sheetId="1" r:id="rId1"/>
-    <sheet name="TC_PRODUCTS_002" sheetId="2" r:id="rId2"/>
-    <sheet name="TC_PRODUCTS_004" sheetId="3" r:id="rId3"/>
-    <sheet name="TC_PRODUCTS_005" sheetId="4" r:id="rId4"/>
-    <sheet name="TC_PRODUCTS_006" sheetId="5" r:id="rId5"/>
-    <sheet name="TC_PRODUCTS_007" sheetId="6" r:id="rId6"/>
-    <sheet name="TC_PRODUCTS_008" sheetId="7" r:id="rId7"/>
-    <sheet name="TC_PRODUCTS_009" sheetId="8" r:id="rId8"/>
+    <sheet name="creationData" sheetId="12" r:id="rId1"/>
+    <sheet name="TC_PRODUCTS_001" sheetId="1" r:id="rId2"/>
+    <sheet name="TC_PRODUCTS_002" sheetId="2" r:id="rId3"/>
+    <sheet name="TC_PRODUCTS_004" sheetId="3" r:id="rId4"/>
+    <sheet name="TC_PRODUCTS_005" sheetId="4" r:id="rId5"/>
+    <sheet name="TC_PRODUCTS_006" sheetId="5" r:id="rId6"/>
+    <sheet name="TC_PRODUCTS_007" sheetId="6" r:id="rId7"/>
+    <sheet name="TC_PRODUCTS_008" sheetId="7" r:id="rId8"/>
+    <sheet name="TC_PRODUCTS_009" sheetId="8" r:id="rId9"/>
+    <sheet name="TC_PRODUCTS_010" sheetId="9" r:id="rId10"/>
+    <sheet name="TC_PRODUCTS_011" sheetId="13" r:id="rId11"/>
+    <sheet name="TC_PRODUCTS_013" sheetId="14" r:id="rId12"/>
+    <sheet name="TC_PRODUCTS_015" sheetId="11" r:id="rId13"/>
+    <sheet name="TC_PRODUCTS_018" sheetId="15" r:id="rId14"/>
+    <sheet name="TC_PRODUCTS_020" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>BreadCrumbsList</t>
   </si>
@@ -129,13 +136,7 @@
     <t>Product Removal Success Message</t>
   </si>
   <si>
-    <t>AutomationProduct3313</t>
-  </si>
-  <si>
     <t>New Product saved successfully</t>
-  </si>
-  <si>
-    <t>AutomationProduct3313 Updated</t>
   </si>
   <si>
     <t>Updated Successfully</t>
@@ -179,12 +180,129 @@
       <t>(Asterisk has to be inculded for mandatory fields)</t>
     </r>
   </si>
+  <si>
+    <t>Product Image Description</t>
+  </si>
+  <si>
+    <t>Product Image URL</t>
+  </si>
+  <si>
+    <t>Product Image success Message</t>
+  </si>
+  <si>
+    <t>Product Image URL saved Successfully</t>
+  </si>
+  <si>
+    <t>http://imaging.nikon.com/lineup/lens/zoom/normalzoom/af-s_dx_18-300mmf_35-56g_ed_vr/img/sample/sample1_l.jpg</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>welcome Message</t>
+  </si>
+  <si>
+    <t>automationUser</t>
+  </si>
+  <si>
+    <t>unilog123##</t>
+  </si>
+  <si>
+    <t>Welcome, Automation !</t>
+  </si>
+  <si>
+    <t>Failed Product Search Message</t>
+  </si>
+  <si>
+    <t>No results Found</t>
+  </si>
+  <si>
+    <t>AutomationTest Image</t>
+  </si>
+  <si>
+    <t>Product Image Upload Success Message</t>
+  </si>
+  <si>
+    <t>Product Image saved Successfully</t>
+  </si>
+  <si>
+    <t>Product Image File location</t>
+  </si>
+  <si>
+    <t>C:\Users\rameshwar.j\Pictures\Screenshots\Screenshot.png</t>
+  </si>
+  <si>
+    <t>Product Image Remove Success Message</t>
+  </si>
+  <si>
+    <t>1 Image removed Successfully</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Item assigned to product message
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Do not include the product name in the success message</t>
+    </r>
+  </si>
+  <si>
+    <t>Assigned Items Saved Successfully to Product</t>
+  </si>
+  <si>
+    <t>General Info,Descriptions,Products,Keywords,Documents,Images,Videos,Linked Items,Attributes,Custom Prices, Categorization,Custom Fields,Warehouse,Customer PartNumber,User Review</t>
+  </si>
+  <si>
+    <t>Edit Item Fields</t>
+  </si>
+  <si>
+    <t>Item Part Number</t>
+  </si>
+  <si>
+    <t>Number of Copies</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>AutomationTestItem 3313</t>
+  </si>
+  <si>
+    <t>AutomationTestProduct 2 Updated</t>
+  </si>
+  <si>
+    <t>AutomationTestProduct 2</t>
+  </si>
+  <si>
+    <t>AutomationTestProduct 1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +329,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF008000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -251,10 +397,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -262,8 +412,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -564,6 +733,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -572,6 +846,153 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.5">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="45">
+      <c r="A1" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="71.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="60">
+      <c r="A2" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -590,7 +1011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -617,7 +1038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -645,7 +1066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -673,12 +1094,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,30 +1134,30 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3">
-        <v>3313</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -751,20 +1172,20 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -777,78 +1198,60 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3">
-        <v>3313</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated porducts module to use creation test data from properties file
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ProductsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ProductsModuleTest.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="creationData" sheetId="12" r:id="rId1"/>
-    <sheet name="TC_PRODUCTS_001" sheetId="1" r:id="rId2"/>
+    <sheet name="TC_PRODUCTS_001" sheetId="1" r:id="rId1"/>
+    <sheet name="TC_PRODUCTS_003" sheetId="12" r:id="rId2"/>
     <sheet name="TC_PRODUCTS_002" sheetId="2" r:id="rId3"/>
     <sheet name="TC_PRODUCTS_004" sheetId="3" r:id="rId4"/>
     <sheet name="TC_PRODUCTS_005" sheetId="4" r:id="rId5"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>BreadCrumbsList</t>
   </si>
@@ -194,30 +194,6 @@
   </si>
   <si>
     <t>http://imaging.nikon.com/lineup/lens/zoom/normalzoom/af-s_dx_18-300mmf_35-56g_ed_vr/img/sample/sample1_l.jpg</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>welcome Message</t>
-  </si>
-  <si>
-    <t>automationUser</t>
-  </si>
-  <si>
-    <t>unilog123##</t>
-  </si>
-  <si>
-    <t>Welcome, Automation !</t>
-  </si>
-  <si>
-    <t>Failed Product Search Message</t>
-  </si>
-  <si>
-    <t>No results Found</t>
   </si>
   <si>
     <t>AutomationTest Image</t>
@@ -733,66 +709,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -816,18 +749,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -851,12 +784,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.5">
       <c r="A2" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -879,12 +812,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="45">
       <c r="A1" s="10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -935,12 +868,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="60">
       <c r="A2" s="11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -964,18 +897,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -985,37 +918,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1134,16 +1083,16 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1239,7 +1188,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>25</v>

</xml_diff>